<commit_message>
wind solar only price
</commit_message>
<xml_diff>
--- a/input_files/case_files/BTES_base_case_solar_wind_no_btes.xlsx
+++ b/input_files/case_files/BTES_base_case_solar_wind_no_btes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciawongel/Work/clab_borehole_th_storage/input_files/case_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awongel/Projects/clab_borehole_th_storage/input_files/case_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF85F9FF-40DB-F94D-B59F-80207262C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896EC405-7F18-884D-9839-986EA8BDD7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="640" windowWidth="33960" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="760" windowWidth="33960" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2036,7 +2036,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="B59" t="s">
         <v>82</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
         <v>83</v>

</xml_diff>